<commit_message>
Update Feefo and Review reports for 2025-04-22T06:01:59Z
</commit_message>
<xml_diff>
--- a/data/product_metadata.xlsx
+++ b/data/product_metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Review Count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>NOTHS URL</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Feefo URL</t>
         </is>
@@ -472,12 +477,15 @@
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-running-shoe-tag</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029103&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -495,12 +503,15 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/thechucklingcheesecompany/product/you-re-not-old-you-re-vintage-cheese-beer-hamper</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -518,12 +529,15 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -541,12 +555,15 @@
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/gaamaa/product/semi-precious-birthstone-sterling-silver-bracelet</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1114901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -564,12 +581,15 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -587,12 +607,15 @@
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/myposhshop/product/watercolour-butterflies-print-scarf</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -610,12 +633,15 @@
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/lovetreedesign/product/kids-personalised-dinosaur-varsity-jacket</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -633,12 +659,15 @@
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/madewithlovecardboutique/product/tiffany-blue-luxury-scented-birthday-card</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -656,12 +685,15 @@
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-curb-chain-necklace</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -679,12 +711,15 @@
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -702,12 +737,15 @@
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/qwertybeerbox/product/personalised-craft-beer-christmas-hamper</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1321115&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -725,12 +763,15 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-open-flat-washbag</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -748,12 +789,15 @@
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -771,12 +815,15 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/hurleyburleyman/product/men-s-engraved-clasp-bracelet</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=429696&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -794,12 +841,15 @@
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -817,12 +867,15 @@
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -840,12 +893,15 @@
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mini-round-travel-jewellery-case</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -863,12 +919,15 @@
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -886,12 +945,15 @@
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -909,12 +971,15 @@
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/alphabetinteriors/product/personalised-sleepover-society-bag</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -932,12 +997,15 @@
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/dibor/product/personalised-standing-double-bird-house-with-stake</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=980169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-04-22T06:17:35Z
</commit_message>
<xml_diff>
--- a/data/product_metadata.xlsx
+++ b/data/product_metadata.xlsx
@@ -476,7 +476,11 @@
           <t>Personalised Running Shoe Tag</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ellie Ellie</t>
+        </is>
+      </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
@@ -502,7 +506,11 @@
           <t>You're Not Old, You're Vintage! Cheese And Beer Hamper</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>thechucklingcheesecompany</t>
+        </is>
+      </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
@@ -528,7 +536,11 @@
           <t>Natural Flowers Spring Door Wreath</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dibor</t>
+        </is>
+      </c>
       <c r="D4" t="n">
         <v>2</v>
       </c>
@@ -554,7 +566,11 @@
           <t>Semi Precious Birthstone Sterling Silver Bracelet</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gaamaa</t>
+        </is>
+      </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
@@ -580,7 +596,11 @@
           <t>Personalised Stainless Steel Pizza Cutter</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Oakdene Designs</t>
+        </is>
+      </c>
       <c r="D6" t="n">
         <v>2</v>
       </c>
@@ -606,7 +626,11 @@
           <t>Delicate Tree Print Scarf</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>My Posh Shop</t>
+        </is>
+      </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
@@ -632,7 +656,11 @@
           <t>Kids Personalised Dinosaur Varsity Jacket</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>lovetreedesign</t>
+        </is>
+      </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
@@ -658,7 +686,11 @@
           <t>Tiffany Blue Luxury Scented Birthday Card</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>madewithlovecardboutique</t>
+        </is>
+      </c>
       <c r="D9" t="n">
         <v>2</v>
       </c>
@@ -684,7 +716,11 @@
           <t>Sterling Silver Light Curb Chain Necklace</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>songsofinkandsteel</t>
+        </is>
+      </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
@@ -710,7 +746,11 @@
           <t>Bunny In A Box</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>thegourmetchocolatepizzaco</t>
+        </is>
+      </c>
       <c r="D11" t="n">
         <v>4</v>
       </c>
@@ -736,7 +776,11 @@
           <t>Personalised Craft Beer Christmas Hamper</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>qwertybeerbox</t>
+        </is>
+      </c>
       <c r="D12" t="n">
         <v>2</v>
       </c>
@@ -762,7 +806,11 @@
           <t>Personalised Open Flat Washbag</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>The Alphabet Gift Shop</t>
+        </is>
+      </c>
       <c r="D13" t="n">
         <v>2</v>
       </c>
@@ -788,7 +836,11 @@
           <t>Personalised Friends With Wine Pebble Picture</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ladedaliving</t>
+        </is>
+      </c>
       <c r="D14" t="n">
         <v>2</v>
       </c>
@@ -814,7 +866,11 @@
           <t>Men's Personalised Engraved Plaited Leather Bracelet</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hurleyburley man</t>
+        </is>
+      </c>
       <c r="D15" t="n">
         <v>2</v>
       </c>
@@ -840,7 +896,11 @@
           <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Joy by Corrine Smith</t>
+        </is>
+      </c>
       <c r="D16" t="n">
         <v>3</v>
       </c>
@@ -866,7 +926,11 @@
           <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>The Rustic Dish®</t>
+        </is>
+      </c>
       <c r="D17" t="n">
         <v>2</v>
       </c>
@@ -892,7 +956,11 @@
           <t>Personalised Mini Round Travel Jewellery Case</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Lisa Angel</t>
+        </is>
+      </c>
       <c r="D18" t="n">
         <v>2</v>
       </c>
@@ -918,7 +986,11 @@
           <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>The Forest &amp; Co</t>
+        </is>
+      </c>
       <c r="D19" t="n">
         <v>2</v>
       </c>
@@ -944,7 +1016,11 @@
           <t>Personalised Leather And Silver St Christopher Bracelet</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Hurleyburley man</t>
+        </is>
+      </c>
       <c r="D20" t="n">
         <v>2</v>
       </c>
@@ -970,7 +1046,11 @@
           <t>Personalised Sleepover Weekend Bag</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>alphabetinteriors</t>
+        </is>
+      </c>
       <c r="D21" t="n">
         <v>2</v>
       </c>
@@ -996,7 +1076,11 @@
           <t>Vintage Standing Heart Garden Bird Feeder</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Dibor</t>
+        </is>
+      </c>
       <c r="D22" t="n">
         <v>2</v>
       </c>

</xml_diff>